<commit_message>
created sqwave library and changed arduino code to include that and test it
</commit_message>
<xml_diff>
--- a/ESE 499 laser characteristics.xlsx
+++ b/ESE 499 laser characteristics.xlsx
@@ -9,17 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22800" windowHeight="8844" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22800" windowHeight="8844" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="3ohm resistor" sheetId="2" r:id="rId2"/>
+    <sheet name="lens calculations" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v3.0" hidden="1">Sheet1!$B$2:$B$58</definedName>
-    <definedName name="_xlchart.v3.1" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v3.2" hidden="1">Sheet1!$D$2:$D$58</definedName>
-    <definedName name="_xlchart.v3.3" hidden="1">Sheet1!$D$2:$D$58</definedName>
-  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -30,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Voltage (mV)</t>
   </si>
@@ -61,18 +57,98 @@
   <si>
     <t>Voltage across Vds</t>
   </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Vx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vin </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I </t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>156u</t>
+  </si>
+  <si>
+    <t>421u</t>
+  </si>
+  <si>
+    <t>839u</t>
+  </si>
+  <si>
+    <t>1.584m</t>
+  </si>
+  <si>
+    <t>3.28m</t>
+  </si>
+  <si>
+    <t>82.4m</t>
+  </si>
+  <si>
+    <t>285m</t>
+  </si>
+  <si>
+    <t>484m</t>
+  </si>
+  <si>
+    <t>687m</t>
+  </si>
+  <si>
+    <t>increased  the opamp to 15</t>
+  </si>
+  <si>
+    <t>Object Distance(u)</t>
+  </si>
+  <si>
+    <t>Image Distance(v)</t>
+  </si>
+  <si>
+    <t>Magnification</t>
+  </si>
+  <si>
+    <t>Focal length</t>
+  </si>
+  <si>
+    <t>Diameter of fiber(Df)</t>
+  </si>
+  <si>
+    <t>Diameter of target(Ds)</t>
+  </si>
+  <si>
+    <t>Umax</t>
+  </si>
+  <si>
+    <t>Radius of lens = 9.14                Divergence angle = 12.709                 (all calculation in mm)</t>
+  </si>
+  <si>
+    <t>Temperature of fet</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -96,8 +172,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1680,6 +1760,406 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Vin</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs I</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'3ohm resistor'!$A$2:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'3ohm resistor'!$B$2:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.156</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.46600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.61799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.77100000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.92500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.077</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.377</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.528</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.68</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.82</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.97</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.125</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.27</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0EEA-458A-8918-C6AE184FDDF7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="150838847"/>
+        <c:axId val="82727455"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="150838847"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="82727455"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="82727455"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="150838847"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1720,7 +2200,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2341,6 +3377,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{740B7DC1-AE24-4A8B-BD37-2F33773155D8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2673,9 +3750,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+    <sheetView zoomScale="79" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3469,4 +4546,610 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="16.8984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0.5</v>
+      </c>
+      <c r="B2">
+        <v>0.156</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>27.8</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <f>G2*3.3</f>
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>31.24</v>
+      </c>
+      <c r="G3">
+        <v>1.5</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H10" si="0">G3*3.3</f>
+        <v>4.9499999999999993</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1.5</v>
+      </c>
+      <c r="B4">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <v>33.92</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>37.44</v>
+      </c>
+      <c r="G5">
+        <v>2.5</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2.5</v>
+      </c>
+      <c r="B6">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6">
+        <v>40.26</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>9.8999999999999986</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>43</v>
+      </c>
+      <c r="G7">
+        <v>3.5</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>11.549999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>3.5</v>
+      </c>
+      <c r="B8">
+        <v>1.077</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8">
+        <v>44.22</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>1.22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9">
+        <v>44.74</v>
+      </c>
+      <c r="G9">
+        <v>4.5</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>14.85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>4.5</v>
+      </c>
+      <c r="B10">
+        <v>1.377</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10">
+        <v>44.7</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>1.528</v>
+      </c>
+      <c r="C11">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="D11">
+        <v>47</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>5.5</v>
+      </c>
+      <c r="B12">
+        <v>1.68</v>
+      </c>
+      <c r="C12">
+        <v>1.08</v>
+      </c>
+      <c r="D12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>1.82</v>
+      </c>
+      <c r="C13">
+        <v>1.2769999999999999</v>
+      </c>
+      <c r="D13">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>6.5</v>
+      </c>
+      <c r="B14">
+        <v>1.97</v>
+      </c>
+      <c r="C14">
+        <v>1.468</v>
+      </c>
+      <c r="D14">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>2.125</v>
+      </c>
+      <c r="C15">
+        <v>1.67</v>
+      </c>
+      <c r="D15">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>7.5</v>
+      </c>
+      <c r="B16">
+        <v>2.27</v>
+      </c>
+      <c r="C16">
+        <v>1.84</v>
+      </c>
+      <c r="D16">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>11.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.69921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6">
+        <v>63.65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <f>A10/B7</f>
+        <v>22.727272727272727</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <f>B$10*C10</f>
+        <v>181.81818181818181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ref="D11:D22" si="0">B$10*C11</f>
+        <v>227.27272727272725</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>340.90909090909088</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>20</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>454.5454545454545</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>25</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>568.18181818181813</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>30</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>681.81818181818176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>35</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>795.45454545454538</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>40</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>909.09090909090901</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>45</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>1022.7272727272727</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>50</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>1136.3636363636363</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>55</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <v>60</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>1363.6363636363635</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>63</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>1431.8181818181818</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>